<commit_message>
RPA Python - Preenchimento de Formulário
</commit_message>
<xml_diff>
--- a/base-preenchimento-de-leads.xlsx
+++ b/base-preenchimento-de-leads.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pedro\Desktop\Estudos\Python - Udemy\Projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44109419-E4FE-4276-831D-BA2C9D4994B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8546F862-77DA-4DE4-A9C1-4D4FD10B24A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1425" windowWidth="29040" windowHeight="15720" xr2:uid="{76C4FD96-251E-4CC9-87AA-2C3F10D9E238}"/>
+    <workbookView xWindow="-27345" yWindow="2985" windowWidth="17250" windowHeight="8865" xr2:uid="{76C4FD96-251E-4CC9-87AA-2C3F10D9E238}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -540,7 +540,7 @@
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C22" ca="1" si="0">RANDBETWEEN(14991111111,14999999999)</f>
-        <v>14992731819</v>
+        <v>14997825179</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:E22" ca="1" si="1">RANDBETWEEN(0,1)</f>
@@ -557,15 +557,15 @@
       </c>
       <c r="B3" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A3," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>luiz_eduardo@hotmail.com</v>
+        <v>luiz_eduardo@yahoo.com</v>
       </c>
       <c r="C3">
         <f t="shared" ca="1" si="0"/>
-        <v>14999303998</v>
+        <v>14999959863</v>
       </c>
       <c r="D3">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <f t="shared" ca="1" si="1"/>
@@ -582,7 +582,7 @@
       </c>
       <c r="C4">
         <f t="shared" ca="1" si="0"/>
-        <v>14992395749</v>
+        <v>14993028862</v>
       </c>
       <c r="D4">
         <f t="shared" ca="1" si="1"/>
@@ -599,11 +599,11 @@
       </c>
       <c r="B5" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A5," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>guilherme@hotmail.com</v>
+        <v>guilherme@yahoo.com</v>
       </c>
       <c r="C5">
         <f t="shared" ca="1" si="0"/>
-        <v>14994627508</v>
+        <v>14998401668</v>
       </c>
       <c r="D5">
         <f t="shared" ca="1" si="1"/>
@@ -624,7 +624,7 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="0"/>
-        <v>14995196490</v>
+        <v>14997937994</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="1"/>
@@ -641,11 +641,11 @@
       </c>
       <c r="B7" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A7," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>joao@gmail.com</v>
+        <v>joao@yahoo.com</v>
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="0"/>
-        <v>14999589444</v>
+        <v>14994770195</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="1"/>
@@ -662,19 +662,19 @@
       </c>
       <c r="B8" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A8," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>josé@yahoo.com</v>
+        <v>josé@outlook.com</v>
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="0"/>
-        <v>14996807674</v>
+        <v>14995172872</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
@@ -683,11 +683,11 @@
       </c>
       <c r="B9" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A9," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>kelvin@gmail.com</v>
+        <v>kelvin@hotmail.com</v>
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="0"/>
-        <v>14991193896</v>
+        <v>14991266334</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="1"/>
@@ -695,7 +695,7 @@
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
@@ -708,11 +708,11 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="0"/>
-        <v>14992965914</v>
+        <v>14998770044</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="1"/>
@@ -725,11 +725,11 @@
       </c>
       <c r="B11" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A11," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>rogério@yahoo.com</v>
+        <v>rogério@gmail.com</v>
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="0"/>
-        <v>14998404648</v>
+        <v>14992481242</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="1"/>
@@ -750,7 +750,7 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="0"/>
-        <v>14997283798</v>
+        <v>14992638260</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="1"/>
@@ -771,11 +771,11 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="0"/>
-        <v>14992348912</v>
+        <v>14994370905</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="1"/>
@@ -792,7 +792,7 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="0"/>
-        <v>14997647762</v>
+        <v>14992634826</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="1"/>
@@ -800,7 +800,7 @@
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
@@ -809,11 +809,11 @@
       </c>
       <c r="B15" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A15," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>luiza@hotmail.com</v>
+        <v>luiza@outlook.com</v>
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="0"/>
-        <v>14998047477</v>
+        <v>14993718388</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="1"/>
@@ -830,11 +830,11 @@
       </c>
       <c r="B16" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A16," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>luis@outlook.com</v>
+        <v>luis@gmail.com</v>
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="0"/>
-        <v>14999017112</v>
+        <v>14991508527</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="1"/>
@@ -842,7 +842,7 @@
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
@@ -855,15 +855,15 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="0"/>
-        <v>14998909695</v>
+        <v>14994303005</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
@@ -872,11 +872,11 @@
       </c>
       <c r="B18" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A18," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>rafael@outlook.com</v>
+        <v>rafael@yahoo.com</v>
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="0"/>
-        <v>14995894118</v>
+        <v>14997332288</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="1"/>
@@ -884,7 +884,7 @@
       </c>
       <c r="E18">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
@@ -893,19 +893,19 @@
       </c>
       <c r="B19" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A19," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>maria_eduarda@hotmail.com</v>
+        <v>maria_eduarda@yahoo.com</v>
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="0"/>
-        <v>14994563472</v>
+        <v>14993276022</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -914,19 +914,19 @@
       </c>
       <c r="B20" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A20," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>maria_luiza@yahoo.com</v>
+        <v>maria_luiza@outlook.com</v>
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="0"/>
-        <v>14995772491</v>
+        <v>14993021713</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -935,19 +935,19 @@
       </c>
       <c r="B21" t="str">
         <f ca="1">_xlfn.CONCAT(LOWER(SUBSTITUTE(A21," ","_")),"@",VLOOKUP(RANDBETWEEN(1,4),Planilha2!A:B,2,0))</f>
-        <v>maria_julia@outlook.com</v>
+        <v>maria_julia@gmail.com</v>
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="0"/>
-        <v>14999785616</v>
+        <v>14991301661</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
@@ -960,15 +960,15 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="0"/>
-        <v>14999330731</v>
+        <v>14998152594</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="1"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>